<commit_message>
modified timesheet of Jason and 2nd meeting minutes
</commit_message>
<xml_diff>
--- a/Time sheet/Timetsheet - Ng Yiu Yeung.xlsx
+++ b/Time sheet/Timetsheet - Ng Yiu Yeung.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/MCI_2021/MCI_Project/Team-024/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A1ADA72-E423-0C42-BC15-5E981C5AD1F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6806C245-D3F9-A84F-BD91-FE95FD8D13BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="500" windowWidth="32800" windowHeight="20000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 2 " sheetId="3" r:id="rId1"/>
     <sheet name="Week 3" sheetId="1" r:id="rId2"/>
     <sheet name="Week 4" sheetId="6" r:id="rId3"/>
     <sheet name="Week 5" sheetId="7" r:id="rId4"/>
+    <sheet name="Week 6" sheetId="8" r:id="rId5"/>
+    <sheet name="Week 7" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 2 '!$A$1:$H$13</definedName>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="70">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -225,6 +227,39 @@
   </si>
   <si>
     <t>Next client meeting</t>
+  </si>
+  <si>
+    <t>Group Meeting</t>
+  </si>
+  <si>
+    <t>Development of Django database</t>
+  </si>
+  <si>
+    <t>Code review and docker &amp; django demonstration</t>
+  </si>
+  <si>
+    <t>Homepage emotion circles resize</t>
+  </si>
+  <si>
+    <t>A key page of the app</t>
+  </si>
+  <si>
+    <t>Review with team mates in the meeting on Sat</t>
+  </si>
+  <si>
+    <t>Complete another 20 % of the ionic course section 6</t>
+  </si>
+  <si>
+    <t>Complete 40% of the ionic course section 6</t>
+  </si>
+  <si>
+    <t>Homepage emotion circles resize (CSS part)</t>
+  </si>
+  <si>
+    <t>Homepage emotion circles resize(Angular JS part)</t>
+  </si>
+  <si>
+    <t>Review with team mates in the meeting on next Sat</t>
   </si>
 </sst>
 </file>
@@ -417,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -505,6 +540,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1832,8 +1870,8 @@
   </sheetPr>
   <dimension ref="A2:AW12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2317,7 +2355,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2805,4 +2843,434 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E57F0CE-B4FB-2848-8FF7-4DF110FCC13C}">
+  <dimension ref="A2:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" customWidth="1"/>
+    <col min="8" max="8" width="56.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E6" s="12">
+        <v>7</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="12">
+        <v>7</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E9" s="12">
+        <v>7</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E6:E11)</f>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{C52136D9-AA38-5745-8110-13F59F39BC3E}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BED0FBF-09B1-214C-9758-E9BC473106E7}">
+  <dimension ref="A2:H12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="8" max="8" width="43.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="12">
+        <v>8</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E10" s="12">
+        <v>8</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="12">
+        <v>5</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E6:E11)</f>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{FEA45DED-71BB-4045-98C0-DF3918D5368D}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>